<commit_message>
added some more plots
</commit_message>
<xml_diff>
--- a/plots/ml_description_by_data_type.xlsx
+++ b/plots/ml_description_by_data_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\literature_review\plots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\literature_review\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CE82B2-D056-438F-A54C-8D32B7AFFE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE6CF84-B4C2-4761-B635-C4D7229A85B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1230" yWindow="-18525" windowWidth="28800" windowHeight="15435" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
+    <workbookView minimized="1" xWindow="2652" yWindow="1080" windowWidth="23040" windowHeight="12120" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -203,7 +203,7 @@
                     <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -316,7 +316,7 @@
                     <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -432,7 +432,7 @@
                     <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -537,7 +537,7 @@
                 <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2125652192"/>
@@ -604,7 +604,7 @@
                 <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2125651360"/>
@@ -643,7 +643,7 @@
               <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -680,7 +680,7 @@
           <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1589,16 +1589,16 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="131" zoomScaleNormal="109" zoomScaleSheetLayoutView="131" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="31.2" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1610,7 +1610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="46.8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="78" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>